<commit_message>
add pdf resume link
</commit_message>
<xml_diff>
--- a/_cv_data/cv_entries.xlsx
+++ b/_cv_data/cv_entries.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>type</t>
   </si>
@@ -515,8 +515,8 @@
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3">
-        <v>2017.0</v>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>18</v>
@@ -644,7 +644,7 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="2"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>

</xml_diff>

<commit_message>
fix digit in the xls file
</commit_message>
<xml_diff>
--- a/_cv_data/cv_entries.xlsx
+++ b/_cv_data/cv_entries.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>type</t>
   </si>
@@ -55,6 +55,9 @@
     <t>education</t>
   </si>
   <si>
+    <t>2019</t>
+  </si>
+  <si>
     <t>Present</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>Flatiron school New York</t>
   </si>
   <si>
+    <t>2002</t>
+  </si>
+  <si>
     <t>2007</t>
   </si>
   <si>
@@ -86,9 +92,6 @@
   </si>
   <si>
     <t>work</t>
-  </si>
-  <si>
-    <t>2019</t>
   </si>
   <si>
     <t>Software Engineer</t>
@@ -213,11 +216,11 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -487,485 +490,485 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
-        <v>2019.0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3">
-        <v>2002.0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2019.0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2018.0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="5"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="E14" s="3"/>
       <c r="F14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I14" s="3"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="2"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="5"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>